<commit_message>
Update Baseline model performance matrix_SAM.xlsx
</commit_message>
<xml_diff>
--- a/Baseline model performance matrix_SAM.xlsx
+++ b/Baseline model performance matrix_SAM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soumavadey/Documents/CS598_DLH/final project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc425df21c088552/Documents/GitHub/COVID-19-CHEST-X-RAY-IMAGE-CLASSISICATION/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{472628A1-4186-234F-A844-3939A7DCA768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{472628A1-4186-234F-A844-3939A7DCA768}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7DD8F60D-0A27-4DB1-B2B1-A876C9636C0F}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5372D0ED-CE0A-944B-84C9-250E41CD4459}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>Model</t>
   </si>
@@ -68,6 +68,22 @@
   </si>
   <si>
     <t>Yet to be done</t>
+  </si>
+  <si>
+    <t>Team Member</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Arjun</t>
+  </si>
+  <si>
+    <t>VGG16</t>
+  </si>
+  <si>
+    <t>Yes(Resize, RandomResizeCrop,
+Horizontal and vertical flip,Rotation and Gaussian Blur)  Requires_grad=False</t>
   </si>
 </sst>
 </file>
@@ -431,21 +447,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77796C96-1636-3D48-81BE-56F810589849}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="74.1640625" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.2890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -461,8 +478,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -478,8 +498,11 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.8">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -495,8 +518,11 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -512,8 +538,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="80" x14ac:dyDescent="0.8">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -529,8 +558,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -546,8 +578,11 @@
       <c r="E6">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="80" x14ac:dyDescent="0.8">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -563,8 +598,11 @@
       <c r="E7">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="80" x14ac:dyDescent="0.8">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -580,8 +618,11 @@
       <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="80" x14ac:dyDescent="0.8">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -597,8 +638,11 @@
       <c r="E9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.8">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -613,6 +657,135 @@
       </c>
       <c r="E10">
         <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.8">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0.66381987577599999</v>
+      </c>
+      <c r="D11">
+        <v>0.97699999999999998</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.8">
+      <c r="A12" t="str">
+        <f>A11</f>
+        <v>SimpleCNN_SAM</v>
+      </c>
+      <c r="B12" t="str">
+        <f>B11</f>
+        <v>Yes(Resize, RandomResizeCrop,
+Horizontal and vertical flip,Rotation and Gaussian Blur)</v>
+      </c>
+      <c r="C12">
+        <v>0.66381987570000001</v>
+      </c>
+      <c r="D12">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.8">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>0.66537000000000002</v>
+      </c>
+      <c r="D13">
+        <v>0.94</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.8">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>0.71273291925465798</v>
+      </c>
+      <c r="D14">
+        <v>0.86329871416091897</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.8">
+      <c r="A15" t="str">
+        <f>A14</f>
+        <v>VGG16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0.78649068322981297</v>
+      </c>
+      <c r="D15">
+        <v>0.76341283321380604</v>
+      </c>
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15" t="str">
+        <f>F14</f>
+        <v>Arjun</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.8">
+      <c r="A16" t="str">
+        <f>A15</f>
+        <v>VGG16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.75</v>
+      </c>
+      <c r="D16">
+        <v>0.70205193758010798</v>
+      </c>
+      <c r="E16">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>